<commit_message>
delete old rsnn materials
</commit_message>
<xml_diff>
--- a/docs/bio/docs.xlsx
+++ b/docs/bio/docs.xlsx
@@ -11,7 +11,7 @@
     <sheet name="docs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">docs!$D$1:$D$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">docs!$D$1:$D$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -38,25 +38,13 @@
     <t xml:space="preserve">locked</t>
   </si>
   <si>
-    <t xml:space="preserve">thesis-body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thesis Body</t>
+    <t xml:space="preserve">cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curriculum Vitae</t>
   </si>
   <si>
     <t xml:space="preserve">Biographical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thesis-slides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thesis Slides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curriculum Vitae</t>
   </si>
   <si>
     <t xml:space="preserve">sop</t>
@@ -192,13 +180,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.66"/>
@@ -250,40 +238,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>